<commit_message>
used dashed lines for optional steps
</commit_message>
<xml_diff>
--- a/fig/typology-flowchart.xlsx
+++ b/fig/typology-flowchart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason.brunson/Documents/research/tahda/imsr/fig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B782D893-0D97-9146-97D1-9516072C6FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D9C90E-F000-D54B-90F9-98C3DFBD193B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16520" yWindow="4360" windowWidth="28040" windowHeight="17440" xr2:uid="{4E28D78B-A5F8-3448-BD2F-2E71EDA01372}"/>
   </bookViews>
@@ -284,6 +284,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
@@ -337,6 +338,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
@@ -390,6 +392,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
@@ -442,7 +445,9 @@
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="25400"/>
+        <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -494,6 +499,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:headEnd type="triangle" w="lg" len="lg"/>
           <a:tailEnd type="none" w="lg" len="lg"/>
         </a:ln>
@@ -548,6 +554,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:headEnd type="triangle" w="lg" len="lg"/>
           <a:tailEnd type="none" w="lg" len="lg"/>
         </a:ln>
@@ -602,6 +609,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:headEnd type="none" w="lg" len="lg"/>
           <a:tailEnd type="none" w="lg" len="lg"/>
         </a:ln>
@@ -818,6 +826,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="25400">
+          <a:prstDash val="sysDash"/>
           <a:headEnd type="triangle" w="lg" len="lg"/>
           <a:tailEnd type="none" w="lg" len="lg"/>
         </a:ln>
@@ -1142,7 +1151,7 @@
   <dimension ref="B1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>